<commit_message>
bug sur l'affichage des charts
</commit_message>
<xml_diff>
--- a/documents/statistiques/Statistiques_M2_2015.xlsx
+++ b/documents/statistiques/Statistiques_M2_2015.xlsx
@@ -74,7 +74,7 @@
     <t>C#</t>
   </si>
   <si>
-    <t>80 %</t>
+    <t>73.33 %</t>
   </si>
   <si>
     <t>COBOL</t>
@@ -412,7 +412,7 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -421,7 +421,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1124,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
@@ -1157,10 +1157,10 @@
         <v>22</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7">

</xml_diff>